<commit_message>
Revert "Revert "first commit""
This reverts commit 92ca77a64713327ac185cfcfc5fb68e630e01af7.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ucc/Documents/GitHub/EXCEL-TEST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F86DB86C-7F5D-0D4F-826C-AFEC145C6733}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9186517A-7F64-E345-B496-6301F1D6373D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{15F9DDA0-FC05-8344-978C-97FB8DBB1A7E}"/>
   </bookViews>
@@ -371,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAF563A-5535-434D-BD13-12F7B4F847CF}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -404,6 +404,31 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="D9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="E10">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Revert "Second Commit""
This reverts commit 43bb3f90849a734cf865bfda7387ca2034f063ec.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ucc/Documents/GitHub/EXCEL-TEST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9186517A-7F64-E345-B496-6301F1D6373D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CD7760-5D94-E743-9A77-74669B56D758}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{15F9DDA0-FC05-8344-978C-97FB8DBB1A7E}"/>
   </bookViews>
@@ -371,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAF563A-5535-434D-BD13-12F7B4F847CF}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A11" sqref="A11:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -429,6 +429,31 @@
         <v>5</v>
       </c>
     </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="D14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="E15">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>